<commit_message>
Atualização automática de NOVO_HAMBURGO.xlsx
</commit_message>
<xml_diff>
--- a/NOVO_HAMBURGO.xlsx
+++ b/NOVO_HAMBURGO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CEB1307-25B1-489E-8288-C16A00436332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE438344-EC2D-4BB4-9789-484E2A3E469C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1142,7 +1129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1202,36 +1189,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1270,14 +1233,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1333,7 +1291,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{FBB31E0A-853C-4775-9171-B161E3EF9B25}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{82D4E25E-D836-4C91-9438-2AC06C389926}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1363,10 +1321,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A16F0530-F611-4F8F-8C43-C5611DBCF8E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38C198B6-722E-42F5-8443-D9DC07A5D87F}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1404,7 +1362,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{501AEFA3-E9C7-402B-99C7-A451BFAB870D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD5AB79-B77A-4DBA-BF65-A2F22958DB0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1467,7 +1425,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A553C01-3B97-4288-A365-6029753B05AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{370C2007-B829-459F-AC0C-E95A09487D3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1486,7 +1444,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31C0A233-B211-2836-AF43-83EE7B0B0FBC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52C1B40E-66C5-BC35-E609-33370B3F591B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1535,7 +1493,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{961105F5-6DB3-7A01-5E97-650608ECC5E5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0B55678-2874-72F2-AAA7-18F5DA9D5D5D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1554,7 +1512,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B4D616-0C6D-29E7-217D-8C12330554EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C95F8F8C-91B7-8FB8-E761-AFDCEFE1F500}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1585,7 +1543,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D64A6CF-A93C-F796-BE2F-F65FA5657514}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11007BEE-19CE-AC7D-9ABA-973BB9C2A7AA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1616,7 +1574,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0BA4171-8057-5F16-2642-0C00197AEE03}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6935F90D-79E4-F354-CA8B-937848068322}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1659,7 +1617,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B77263B-663A-4878-968B-F4144F90F39A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1894F57E-33BE-4DB7-8BB1-877B56AC6ABC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1697,7 +1655,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DC929B8-7EEC-47BA-840F-0D856B82D84D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB63DF5-A2FE-4F89-B0F1-164119CE66A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1740,7 +1698,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE92178-64CB-4A69-A6F4-94CBCF9E1D6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66E72958-E879-458A-A573-C28C0D3AC156}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2053,7 +2011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBE83CB-0CBE-49FB-AB1A-16CD401ACFD9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15818879-2972-4C59-8027-F8D18D5774A2}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2065,98 +2023,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5486,19 +5444,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5521,90 +5479,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>288</v>
       </c>
     </row>
@@ -5622,16 +5580,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5665,7 +5623,7 @@
       <c r="J1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="21" t="s">
         <v>298</v>
       </c>
     </row>
@@ -5679,10 +5637,10 @@
       <c r="C2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="22">
         <v>169</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>16.899999999999999</v>
       </c>
       <c r="F2" s="2">
@@ -5700,7 +5658,7 @@
       <c r="J2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="23">
         <v>704</v>
       </c>
     </row>
@@ -5725,54 +5683,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>319</v>
       </c>
     </row>
@@ -5783,41 +5742,41 @@
       <c r="B2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45870</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>76109</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>9323</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="31" t="s">
         <v>324</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>324</v>
       </c>
     </row>
@@ -5848,25 +5807,24 @@
       <c r="B1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="36">
         <v>222</v>
       </c>
-      <c r="F1" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>299</v>
-      </c>
-      <c r="B2" s="39">
-        <v>222</v>
-      </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>1.468059780452321E-2</v>
       </c>
     </row>

</xml_diff>